<commit_message>
Finished trailer conflict basic scenes
</commit_message>
<xml_diff>
--- a/Assets/Trailer_2/timeline.xlsx
+++ b/Assets/Trailer_2/timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cursed Silence\Trailer 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\Horror_FPS\Assets\Trailer_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050586C4-D6B0-4979-99A1-7EC48351F324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AED52D-E533-41FD-B6F0-15299B365F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>UNION</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>running (carry)</t>
+  </si>
+  <si>
+    <t>scene 18 make him falling down (see if better or already down suffering better)</t>
+  </si>
+  <si>
+    <t>Line when seeing diary: I won't read it ever again</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -486,9 +492,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,9 +500,108 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,105 +612,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:AE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,30 +919,30 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="19">
         <v>0</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="25">
+      <c r="I5" s="19">
         <v>1.6666666666666667</v>
       </c>
-      <c r="J5" s="26"/>
+      <c r="J5" s="20"/>
       <c r="K5" s="2"/>
       <c r="L5" s="4"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="25">
+      <c r="Q5" s="19">
         <v>5.486111111111111E-2</v>
       </c>
-      <c r="R5" s="26"/>
+      <c r="R5" s="20"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
@@ -947,107 +950,107 @@
       <c r="W5" s="3"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="25">
+      <c r="Z5" s="19">
         <v>7.9861111111111105E-2</v>
       </c>
-      <c r="AA5" s="25"/>
+      <c r="AA5" s="19"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
-      <c r="AD5" s="25">
+      <c r="AD5" s="19">
         <v>9.5833333333333326E-2</v>
       </c>
-      <c r="AE5" s="26"/>
+      <c r="AE5" s="20"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="33" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="36" t="s">
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
-      <c r="Y6" s="37"/>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="27" t="s">
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="32"/>
+      <c r="AA6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AB6" s="28"/>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="29"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="23"/>
       <c r="AE6" s="2"/>
     </row>
     <row r="7" spans="1:31" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="49" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="46" t="s">
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="44" t="s">
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="41" t="s">
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="39" t="s">
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="39"/>
-      <c r="X7" s="39"/>
-      <c r="Y7" s="39"/>
-      <c r="Z7" s="40"/>
-      <c r="AA7" s="23" t="s">
+      <c r="W7" s="33"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="24"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="18"/>
       <c r="AE7" s="2"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1078,7 +1081,7 @@
       <c r="I8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1087,104 +1090,104 @@
       <c r="L8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="P8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="R8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="U8" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="V8" s="11" t="s">
+      <c r="V8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="W8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="X8" s="12" t="s">
+      <c r="X8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="Y8" s="12" t="s">
+      <c r="Y8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="Z8" s="12" t="s">
+      <c r="Z8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AA8" s="51" t="s">
+      <c r="AA8" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="51" t="s">
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AD8" s="52"/>
+      <c r="AD8" s="47"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17" t="s">
+      <c r="C9" s="48"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17" t="s">
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17" t="s">
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17" t="s">
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="18" t="s">
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="19" t="s">
+      <c r="W9" s="50"/>
+      <c r="X9" s="50"/>
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="50"/>
+      <c r="AA9" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="51"/>
+      <c r="AD9" s="51"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1246,20 +1249,20 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="15"/>
+      <c r="J11" s="45"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="R11" s="15"/>
+      <c r="R11" s="45"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -1273,13 +1276,24 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="19" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>56</v>
       </c>
+      <c r="N19" s="13"/>
     </row>
     <row r="20" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="V20" s="14"/>
+      <c r="V20" s="13"/>
     </row>
     <row r="21" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -1324,12 +1338,12 @@
       </c>
     </row>
     <row r="27" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="28" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1340,6 +1354,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="V9:Z9"/>
+    <mergeCell ref="AA9:AD9"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="AA7:AD7"/>
     <mergeCell ref="AD5:AE5"/>
@@ -1356,17 +1381,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="N9:Q9"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="V9:Z9"/>
-    <mergeCell ref="AA9:AD9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>